<commit_message>
Updated baseline coverage of fortification to give the correct total budget
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Tanzania/2017Sep/InputForCode_Tanzania_FortificationOnly.xlsx
+++ b/input_spreadsheets/Tanzania/2017Sep/InputForCode_Tanzania_FortificationOnly.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="11" activeTab="20"/>
+    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="15" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -787,6 +787,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author xml:space="preserve"> Janka Petravic</author>
+    <author>Sam</author>
   </authors>
   <commentList>
     <comment ref="D3" authorId="0">
@@ -874,6 +875,28 @@
           </rPr>
           <t xml:space="preserve">
 Cochrane review - not finished; no who guidelines.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+This is fictional and designed to produce the desired total budget in optimisation</t>
         </r>
       </text>
     </comment>
@@ -1473,7 +1496,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1485,6 +1508,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1594,7 +1619,7 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="59">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1623,6 +1648,7 @@
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1650,6 +1676,7 @@
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
@@ -4807,8 +4834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4920,7 +4947,7 @@
         <v>79</v>
       </c>
       <c r="B7" s="24">
-        <v>0</v>
+        <v>0.92924764559999995</v>
       </c>
       <c r="C7" s="26">
         <v>0.95</v>
@@ -5017,7 +5044,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>

</xml_diff>